<commit_message>
Update work with pandas and start tips and tricks.
</commit_message>
<xml_diff>
--- a/Python_Ka_Chilla/day_6/pandas_01_day6.xlsx
+++ b/Python_Ka_Chilla/day_6/pandas_01_day6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="10">
   <si>
     <t>height</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>Pasta</t>
-  </si>
-  <si>
-    <t>6Ft</t>
-  </si>
-  <si>
-    <t>5.8ft</t>
   </si>
   <si>
     <t>Chapel Kaba</t>
@@ -727,8 +721,8 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="1" t="s">
-        <v>7</v>
+      <c r="A27" s="1">
+        <v>6</v>
       </c>
       <c r="B27" s="2">
         <v>50</v>
@@ -760,8 +754,8 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="1" t="s">
-        <v>8</v>
+      <c r="A30" s="1">
+        <v>5.8</v>
       </c>
       <c r="B30" s="5">
         <v>65</v>
@@ -822,7 +816,7 @@
         <v>103</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15.75">
@@ -833,7 +827,7 @@
         <v>110</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15.75">
@@ -877,7 +871,7 @@
         <v>61</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="15.75">
@@ -948,13 +942,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="15.75">
       <c r="A47" s="5">
-        <v>167</v>
+        <v>5.4</v>
       </c>
       <c r="B47" s="5">
         <v>60</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="15.75">
@@ -987,7 +981,7 @@
         <v>72</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="15.75">
@@ -1014,7 +1008,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="15.75">
       <c r="A53" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B53" s="5">
         <v>68</v>
@@ -1108,7 +1102,7 @@
         <v>51</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="15.75">
@@ -1229,7 +1223,7 @@
         <v>65</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
@@ -1278,13 +1272,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B77" s="5">
         <v>125</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">

</xml_diff>